<commit_message>
add updates to lesson 21 R code
</commit_message>
<xml_diff>
--- a/smallExample.xlsx
+++ b/smallExample.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9975" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9975" windowHeight="2700" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="rmanova1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>How many data points are there?</t>
   </si>
@@ -431,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -584,7 +585,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -986,4 +987,167 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>9.9</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>10.1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>11.7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>11.9</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>3.2</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>3.3</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>3.4</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>5.2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>5.4</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>5.6</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>